<commit_message>
Minor fixes and generate synapseImage
</commit_message>
<xml_diff>
--- a/output/synapseData.xlsx
+++ b/output/synapseData.xlsx
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -625,7 +625,7 @@
         </is>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -919,7 +919,7 @@
         </is>
       </c>
       <c r="E23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="E24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="E28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="E29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1255,7 +1255,7 @@
         </is>
       </c>
       <c r="E39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1486,7 +1486,7 @@
         </is>
       </c>
       <c r="E50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1549,7 +1549,7 @@
         </is>
       </c>
       <c r="E53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1633,7 +1633,7 @@
         </is>
       </c>
       <c r="E57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="E66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2137,7 +2137,7 @@
         </is>
       </c>
       <c r="E81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2305,7 +2305,7 @@
         </is>
       </c>
       <c r="E89" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -2515,7 +2515,7 @@
         </is>
       </c>
       <c r="E99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -2641,7 +2641,7 @@
         </is>
       </c>
       <c r="E105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -3124,7 +3124,7 @@
         </is>
       </c>
       <c r="E128" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -3376,7 +3376,7 @@
         </is>
       </c>
       <c r="E140" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -3586,7 +3586,7 @@
         </is>
       </c>
       <c r="E150" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -3607,7 +3607,7 @@
         </is>
       </c>
       <c r="E151" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -3712,7 +3712,7 @@
         </is>
       </c>
       <c r="E156" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -3880,7 +3880,7 @@
         </is>
       </c>
       <c r="E164" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -3922,7 +3922,7 @@
         </is>
       </c>
       <c r="E166" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -3943,7 +3943,7 @@
         </is>
       </c>
       <c r="E167" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -3985,7 +3985,7 @@
         </is>
       </c>
       <c r="E169" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -4069,7 +4069,7 @@
         </is>
       </c>
       <c r="E173" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -4510,7 +4510,7 @@
         </is>
       </c>
       <c r="E194" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -4531,7 +4531,7 @@
         </is>
       </c>
       <c r="E195" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -4594,7 +4594,7 @@
         </is>
       </c>
       <c r="E198" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -4615,7 +4615,7 @@
         </is>
       </c>
       <c r="E199" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -4762,7 +4762,7 @@
         </is>
       </c>
       <c r="E206" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207">
@@ -4930,7 +4930,7 @@
         </is>
       </c>
       <c r="E214" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215">
@@ -4972,7 +4972,7 @@
         </is>
       </c>
       <c r="E216" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217">
@@ -5056,7 +5056,7 @@
         </is>
       </c>
       <c r="E220" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -5077,7 +5077,7 @@
         </is>
       </c>
       <c r="E221" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222">
@@ -5161,7 +5161,7 @@
         </is>
       </c>
       <c r="E225" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226">
@@ -5182,7 +5182,7 @@
         </is>
       </c>
       <c r="E226" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227">
@@ -5266,7 +5266,7 @@
         </is>
       </c>
       <c r="E230" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231">
@@ -5392,7 +5392,7 @@
         </is>
       </c>
       <c r="E236" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
@@ -5476,7 +5476,7 @@
         </is>
       </c>
       <c r="E240" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241">
@@ -5644,7 +5644,7 @@
         </is>
       </c>
       <c r="E248" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249">
@@ -5665,7 +5665,7 @@
         </is>
       </c>
       <c r="E249" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250">
@@ -5791,7 +5791,7 @@
         </is>
       </c>
       <c r="E255" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256">
@@ -5896,7 +5896,7 @@
         </is>
       </c>
       <c r="E260" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261">
@@ -5917,7 +5917,7 @@
         </is>
       </c>
       <c r="E261" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262">
@@ -6001,7 +6001,7 @@
         </is>
       </c>
       <c r="E265" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266">
@@ -6064,7 +6064,7 @@
         </is>
       </c>
       <c r="E268" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269">
@@ -6085,7 +6085,7 @@
         </is>
       </c>
       <c r="E269" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="270">
@@ -6358,7 +6358,7 @@
         </is>
       </c>
       <c r="E282" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283">
@@ -6379,7 +6379,7 @@
         </is>
       </c>
       <c r="E283" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284">
@@ -6568,7 +6568,7 @@
         </is>
       </c>
       <c r="E292" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="293">
@@ -6694,7 +6694,7 @@
         </is>
       </c>
       <c r="E298" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299">
@@ -6736,7 +6736,7 @@
         </is>
       </c>
       <c r="E300" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301">
@@ -6841,7 +6841,7 @@
         </is>
       </c>
       <c r="E305" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="306">
@@ -7030,7 +7030,7 @@
         </is>
       </c>
       <c r="E314" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="315">
@@ -7051,7 +7051,7 @@
         </is>
       </c>
       <c r="E315" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="316">
@@ -7366,7 +7366,7 @@
         </is>
       </c>
       <c r="E330" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331">
@@ -7429,7 +7429,7 @@
         </is>
       </c>
       <c r="E333" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="334">
@@ -7492,7 +7492,7 @@
         </is>
       </c>
       <c r="E336" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="337">
@@ -7954,7 +7954,7 @@
         </is>
       </c>
       <c r="E358" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359">
@@ -8059,7 +8059,7 @@
         </is>
       </c>
       <c r="E363" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364">
@@ -8521,7 +8521,7 @@
         </is>
       </c>
       <c r="E385" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386">
@@ -8563,7 +8563,7 @@
         </is>
       </c>
       <c r="E387" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="388">
@@ -8710,7 +8710,7 @@
         </is>
       </c>
       <c r="E394" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="395">
@@ -8857,7 +8857,7 @@
         </is>
       </c>
       <c r="E401" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="402">
@@ -8899,7 +8899,7 @@
         </is>
       </c>
       <c r="E403" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="404">
@@ -8962,7 +8962,7 @@
         </is>
       </c>
       <c r="E406" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="407">
@@ -9298,7 +9298,7 @@
         </is>
       </c>
       <c r="E422" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="423">
@@ -9508,7 +9508,7 @@
         </is>
       </c>
       <c r="E432" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="433">
@@ -9634,7 +9634,7 @@
         </is>
       </c>
       <c r="E438" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="439">
@@ -9676,7 +9676,7 @@
         </is>
       </c>
       <c r="E440" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="441">
@@ -9697,7 +9697,7 @@
         </is>
       </c>
       <c r="E441" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="442">
@@ -9718,7 +9718,7 @@
         </is>
       </c>
       <c r="E442" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="443">
@@ -9886,7 +9886,7 @@
         </is>
       </c>
       <c r="E450" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="451">
@@ -9970,7 +9970,7 @@
         </is>
       </c>
       <c r="E454" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="455">
@@ -10096,7 +10096,7 @@
         </is>
       </c>
       <c r="E460" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="461">
@@ -10117,7 +10117,7 @@
         </is>
       </c>
       <c r="E461" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="462">
@@ -10138,7 +10138,7 @@
         </is>
       </c>
       <c r="E462" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="463">
@@ -10222,7 +10222,7 @@
         </is>
       </c>
       <c r="E466" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="467">
@@ -10264,7 +10264,7 @@
         </is>
       </c>
       <c r="E468" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="469">
@@ -10327,7 +10327,7 @@
         </is>
       </c>
       <c r="E471" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="472">
@@ -10411,7 +10411,7 @@
         </is>
       </c>
       <c r="E475" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="476">
@@ -10432,7 +10432,7 @@
         </is>
       </c>
       <c r="E476" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="477">
@@ -10621,7 +10621,7 @@
         </is>
       </c>
       <c r="E485" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="486">
@@ -10684,7 +10684,7 @@
         </is>
       </c>
       <c r="E488" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="489">
@@ -10726,7 +10726,7 @@
         </is>
       </c>
       <c r="E490" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="491">
@@ -10810,7 +10810,7 @@
         </is>
       </c>
       <c r="E494" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="495">
@@ -10894,7 +10894,7 @@
         </is>
       </c>
       <c r="E498" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="499">
@@ -10936,7 +10936,7 @@
         </is>
       </c>
       <c r="E500" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="501">
@@ -11062,7 +11062,7 @@
         </is>
       </c>
       <c r="E506" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="507">
@@ -11083,7 +11083,7 @@
         </is>
       </c>
       <c r="E507" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="508">
@@ -11146,7 +11146,7 @@
         </is>
       </c>
       <c r="E510" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="511">
@@ -11209,7 +11209,7 @@
         </is>
       </c>
       <c r="E513" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="514">
@@ -11251,7 +11251,7 @@
         </is>
       </c>
       <c r="E515" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="516">
@@ -11314,7 +11314,7 @@
         </is>
       </c>
       <c r="E518" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="519">
@@ -11335,7 +11335,7 @@
         </is>
       </c>
       <c r="E519" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="520">
@@ -11419,7 +11419,7 @@
         </is>
       </c>
       <c r="E523" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="524">
@@ -11482,7 +11482,7 @@
         </is>
       </c>
       <c r="E526" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="527">
@@ -11524,7 +11524,7 @@
         </is>
       </c>
       <c r="E528" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="529">
@@ -11587,7 +11587,7 @@
         </is>
       </c>
       <c r="E531" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="532">
@@ -11881,7 +11881,7 @@
         </is>
       </c>
       <c r="E545" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="546">
@@ -11965,7 +11965,7 @@
         </is>
       </c>
       <c r="E549" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="550">
@@ -12028,7 +12028,7 @@
         </is>
       </c>
       <c r="E552" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="553">
@@ -12049,7 +12049,7 @@
         </is>
       </c>
       <c r="E553" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="554">
@@ -12070,7 +12070,7 @@
         </is>
       </c>
       <c r="E554" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="555">
@@ -12133,7 +12133,7 @@
         </is>
       </c>
       <c r="E557" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="558">
@@ -12196,7 +12196,7 @@
         </is>
       </c>
       <c r="E560" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="561">
@@ -12889,7 +12889,7 @@
         </is>
       </c>
       <c r="E593" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="594">
@@ -12952,7 +12952,7 @@
         </is>
       </c>
       <c r="E596" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="597">
@@ -13099,7 +13099,7 @@
         </is>
       </c>
       <c r="E603" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="604">
@@ -13267,7 +13267,7 @@
         </is>
       </c>
       <c r="E611" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="612">
@@ -13309,7 +13309,7 @@
         </is>
       </c>
       <c r="E613" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="614">
@@ -13330,7 +13330,7 @@
         </is>
       </c>
       <c r="E614" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="615">
@@ -13435,7 +13435,7 @@
         </is>
       </c>
       <c r="E619" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="620">
@@ -13582,7 +13582,7 @@
         </is>
       </c>
       <c r="E626" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="627">
@@ -13708,7 +13708,7 @@
         </is>
       </c>
       <c r="E632" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="633">
@@ -13813,7 +13813,7 @@
         </is>
       </c>
       <c r="E637" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="638">
@@ -14233,7 +14233,7 @@
         </is>
       </c>
       <c r="E657" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="658">
@@ -14296,7 +14296,7 @@
         </is>
       </c>
       <c r="E660" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="661">
@@ -14527,7 +14527,7 @@
         </is>
       </c>
       <c r="E671" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="672">
@@ -14590,7 +14590,7 @@
         </is>
       </c>
       <c r="E674" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="675">
@@ -14632,7 +14632,7 @@
         </is>
       </c>
       <c r="E676" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="677">
@@ -14737,7 +14737,7 @@
         </is>
       </c>
       <c r="E681" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="682">
@@ -14758,7 +14758,7 @@
         </is>
       </c>
       <c r="E682" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="683">
@@ -14821,7 +14821,7 @@
         </is>
       </c>
       <c r="E685" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="686">
@@ -14863,7 +14863,7 @@
         </is>
       </c>
       <c r="E687" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="688">
@@ -14926,7 +14926,7 @@
         </is>
       </c>
       <c r="E690" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="691">
@@ -15010,7 +15010,7 @@
         </is>
       </c>
       <c r="E694" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="695">
@@ -15094,7 +15094,7 @@
         </is>
       </c>
       <c r="E698" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="699">
@@ -15241,7 +15241,7 @@
         </is>
       </c>
       <c r="E705" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="706">
@@ -15262,7 +15262,7 @@
         </is>
       </c>
       <c r="E706" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="707">
@@ -15346,7 +15346,7 @@
         </is>
       </c>
       <c r="E710" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="711">
@@ -15367,7 +15367,7 @@
         </is>
       </c>
       <c r="E711" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="712">
@@ -15409,7 +15409,7 @@
         </is>
       </c>
       <c r="E713" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="714">
@@ -15430,7 +15430,7 @@
         </is>
       </c>
       <c r="E714" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="715">
@@ -15535,7 +15535,7 @@
         </is>
       </c>
       <c r="E719" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="720">
@@ -15598,7 +15598,7 @@
         </is>
       </c>
       <c r="E722" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="723">
@@ -15640,7 +15640,7 @@
         </is>
       </c>
       <c r="E724" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="725">
@@ -15808,7 +15808,7 @@
         </is>
       </c>
       <c r="E732" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="733">
@@ -15871,7 +15871,7 @@
         </is>
       </c>
       <c r="E735" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="736">
@@ -15913,7 +15913,7 @@
         </is>
       </c>
       <c r="E737" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="738">
@@ -16039,7 +16039,7 @@
         </is>
       </c>
       <c r="E743" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="744">
@@ -16081,7 +16081,7 @@
         </is>
       </c>
       <c r="E745" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="746">
@@ -16102,7 +16102,7 @@
         </is>
       </c>
       <c r="E746" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="747">
@@ -16228,7 +16228,7 @@
         </is>
       </c>
       <c r="E752" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="753">
@@ -16375,7 +16375,7 @@
         </is>
       </c>
       <c r="E759" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="760">
@@ -16417,7 +16417,7 @@
         </is>
       </c>
       <c r="E761" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="762">
@@ -16459,7 +16459,7 @@
         </is>
       </c>
       <c r="E763" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="764">
@@ -16606,7 +16606,7 @@
         </is>
       </c>
       <c r="E770" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="771">
@@ -16648,7 +16648,7 @@
         </is>
       </c>
       <c r="E772" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="773">
@@ -16921,7 +16921,7 @@
         </is>
       </c>
       <c r="E785" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="786">
@@ -17026,7 +17026,7 @@
         </is>
       </c>
       <c r="E790" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="791">
@@ -17215,7 +17215,7 @@
         </is>
       </c>
       <c r="E799" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="800">
@@ -17488,7 +17488,7 @@
         </is>
       </c>
       <c r="E812" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="813">
@@ -17551,7 +17551,7 @@
         </is>
       </c>
       <c r="E815" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="816">
@@ -17572,7 +17572,7 @@
         </is>
       </c>
       <c r="E816" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="817">
@@ -17698,7 +17698,7 @@
         </is>
       </c>
       <c r="E822" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="823">
@@ -17782,7 +17782,7 @@
         </is>
       </c>
       <c r="E826" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="827">
@@ -17845,7 +17845,7 @@
         </is>
       </c>
       <c r="E829" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="830">
@@ -17929,7 +17929,7 @@
         </is>
       </c>
       <c r="E833" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="834">
@@ -17971,7 +17971,7 @@
         </is>
       </c>
       <c r="E835" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="836">
@@ -18076,7 +18076,7 @@
         </is>
       </c>
       <c r="E840" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="841">
@@ -18139,7 +18139,7 @@
         </is>
       </c>
       <c r="E843" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="844">
@@ -18160,7 +18160,7 @@
         </is>
       </c>
       <c r="E844" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="845">
@@ -18265,7 +18265,7 @@
         </is>
       </c>
       <c r="E849" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="850">
@@ -18286,7 +18286,7 @@
         </is>
       </c>
       <c r="E850" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="851">
@@ -18349,7 +18349,7 @@
         </is>
       </c>
       <c r="E853" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="854">
@@ -18412,7 +18412,7 @@
         </is>
       </c>
       <c r="E856" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="857">
@@ -18643,7 +18643,7 @@
         </is>
       </c>
       <c r="E867" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="868">
@@ -18664,7 +18664,7 @@
         </is>
       </c>
       <c r="E868" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="869">
@@ -18832,7 +18832,7 @@
         </is>
       </c>
       <c r="E876" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="877">
@@ -18874,7 +18874,7 @@
         </is>
       </c>
       <c r="E878" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="879">
@@ -19273,7 +19273,7 @@
         </is>
       </c>
       <c r="E897" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="898">
@@ -19399,7 +19399,7 @@
         </is>
       </c>
       <c r="E903" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="904">
@@ -19525,7 +19525,7 @@
         </is>
       </c>
       <c r="E909" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="910">
@@ -19546,7 +19546,7 @@
         </is>
       </c>
       <c r="E910" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="911">
@@ -19819,7 +19819,7 @@
         </is>
       </c>
       <c r="E923" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="924">
@@ -20008,7 +20008,7 @@
         </is>
       </c>
       <c r="E932" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="933">
@@ -20092,7 +20092,7 @@
         </is>
       </c>
       <c r="E936" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="937">
@@ -20218,7 +20218,7 @@
         </is>
       </c>
       <c r="E942" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="943">
@@ -20386,7 +20386,7 @@
         </is>
       </c>
       <c r="E950" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="951">
@@ -20407,7 +20407,7 @@
         </is>
       </c>
       <c r="E951" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="952">
@@ -20428,7 +20428,7 @@
         </is>
       </c>
       <c r="E952" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="953">
@@ -20491,7 +20491,7 @@
         </is>
       </c>
       <c r="E955" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="956">
@@ -20512,7 +20512,7 @@
         </is>
       </c>
       <c r="E956" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="957">
@@ -20701,7 +20701,7 @@
         </is>
       </c>
       <c r="E965" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="966">
@@ -20974,7 +20974,7 @@
         </is>
       </c>
       <c r="E978" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="979">
@@ -21058,7 +21058,7 @@
         </is>
       </c>
       <c r="E982" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="983">
@@ -21625,7 +21625,7 @@
         </is>
       </c>
       <c r="E1009" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1010">
@@ -21646,7 +21646,7 @@
         </is>
       </c>
       <c r="E1010" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1011">
@@ -21835,7 +21835,7 @@
         </is>
       </c>
       <c r="E1019" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1020">
@@ -22003,7 +22003,7 @@
         </is>
       </c>
       <c r="E1027" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1028">
@@ -22108,7 +22108,7 @@
         </is>
       </c>
       <c r="E1032" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1033">
@@ -22465,7 +22465,7 @@
         </is>
       </c>
       <c r="E1049" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1050">
@@ -22486,7 +22486,7 @@
         </is>
       </c>
       <c r="E1050" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1051">
@@ -22654,7 +22654,7 @@
         </is>
       </c>
       <c r="E1058" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1059">
@@ -22696,7 +22696,7 @@
         </is>
       </c>
       <c r="E1060" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1061">
@@ -22864,7 +22864,7 @@
         </is>
       </c>
       <c r="E1068" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1069">
@@ -23011,7 +23011,7 @@
         </is>
       </c>
       <c r="E1075" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1076">
@@ -23032,7 +23032,7 @@
         </is>
       </c>
       <c r="E1076" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1077">
@@ -23221,7 +23221,7 @@
         </is>
       </c>
       <c r="E1085" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1086">
@@ -23242,7 +23242,7 @@
         </is>
       </c>
       <c r="E1086" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1087">
@@ -23704,7 +23704,7 @@
         </is>
       </c>
       <c r="E1108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1109">
@@ -23725,7 +23725,7 @@
         </is>
       </c>
       <c r="E1109" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1110">
@@ -23746,7 +23746,7 @@
         </is>
       </c>
       <c r="E1110" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1111">
@@ -23767,7 +23767,7 @@
         </is>
       </c>
       <c r="E1111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1112">
@@ -23914,7 +23914,7 @@
         </is>
       </c>
       <c r="E1118" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1119">
@@ -23956,7 +23956,7 @@
         </is>
       </c>
       <c r="E1120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1121">
@@ -24040,7 +24040,7 @@
         </is>
       </c>
       <c r="E1124" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1125">
@@ -24082,7 +24082,7 @@
         </is>
       </c>
       <c r="E1126" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1127">
@@ -24166,7 +24166,7 @@
         </is>
       </c>
       <c r="E1130" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1131">
@@ -24460,7 +24460,7 @@
         </is>
       </c>
       <c r="E1144" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1145">
@@ -24481,7 +24481,7 @@
         </is>
       </c>
       <c r="E1145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1146">
@@ -24628,7 +24628,7 @@
         </is>
       </c>
       <c r="E1152" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1153">
@@ -24691,7 +24691,7 @@
         </is>
       </c>
       <c r="E1155" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1156">
@@ -24775,7 +24775,7 @@
         </is>
       </c>
       <c r="E1159" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1160">
@@ -24922,7 +24922,7 @@
         </is>
       </c>
       <c r="E1166" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1167">
@@ -25006,7 +25006,7 @@
         </is>
       </c>
       <c r="E1170" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1171">
@@ -25027,7 +25027,7 @@
         </is>
       </c>
       <c r="E1171" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1172">
@@ -25069,7 +25069,7 @@
         </is>
       </c>
       <c r="E1173" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1174">
@@ -25111,7 +25111,7 @@
         </is>
       </c>
       <c r="E1175" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1176">
@@ -25279,7 +25279,7 @@
         </is>
       </c>
       <c r="E1183" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1184">
@@ -25657,7 +25657,7 @@
         </is>
       </c>
       <c r="E1201" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1202">
@@ -25846,7 +25846,7 @@
         </is>
       </c>
       <c r="E1210" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1211">
@@ -25867,7 +25867,7 @@
         </is>
       </c>
       <c r="E1211" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1212">
@@ -26056,7 +26056,7 @@
         </is>
       </c>
       <c r="E1220" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1221">
@@ -26182,7 +26182,7 @@
         </is>
       </c>
       <c r="E1226" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1227">
@@ -26266,7 +26266,7 @@
         </is>
       </c>
       <c r="E1230" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1231">
@@ -26329,7 +26329,7 @@
         </is>
       </c>
       <c r="E1233" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1234">
@@ -26350,7 +26350,7 @@
         </is>
       </c>
       <c r="E1234" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1235">
@@ -26371,7 +26371,7 @@
         </is>
       </c>
       <c r="E1235" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1236">
@@ -26476,7 +26476,7 @@
         </is>
       </c>
       <c r="E1240" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1241">
@@ -26497,7 +26497,7 @@
         </is>
       </c>
       <c r="E1241" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1242">
@@ -26560,7 +26560,7 @@
         </is>
       </c>
       <c r="E1244" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1245">
@@ -26812,7 +26812,7 @@
         </is>
       </c>
       <c r="E1256" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1257">
@@ -26833,7 +26833,7 @@
         </is>
       </c>
       <c r="E1257" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1258">
@@ -27022,7 +27022,7 @@
         </is>
       </c>
       <c r="E1266" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1267">
@@ -27358,7 +27358,7 @@
         </is>
       </c>
       <c r="E1282" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1283">
@@ -27505,7 +27505,7 @@
         </is>
       </c>
       <c r="E1289" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1290">
@@ -27610,7 +27610,7 @@
         </is>
       </c>
       <c r="E1294" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1295">
@@ -27652,7 +27652,7 @@
         </is>
       </c>
       <c r="E1296" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1297">
@@ -27736,7 +27736,7 @@
         </is>
       </c>
       <c r="E1300" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1301">
@@ -28114,7 +28114,7 @@
         </is>
       </c>
       <c r="E1318" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1319">
@@ -28156,7 +28156,7 @@
         </is>
       </c>
       <c r="E1320" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1321">
@@ -28366,7 +28366,7 @@
         </is>
       </c>
       <c r="E1330" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1331">
@@ -28492,7 +28492,7 @@
         </is>
       </c>
       <c r="E1336" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1337">
@@ -28618,7 +28618,7 @@
         </is>
       </c>
       <c r="E1342" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1343">
@@ -28765,7 +28765,7 @@
         </is>
       </c>
       <c r="E1349" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1350">
@@ -28807,7 +28807,7 @@
         </is>
       </c>
       <c r="E1351" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1352">
@@ -28849,7 +28849,7 @@
         </is>
       </c>
       <c r="E1353" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1354">
@@ -28933,7 +28933,7 @@
         </is>
       </c>
       <c r="E1357" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1358">
@@ -28975,7 +28975,7 @@
         </is>
       </c>
       <c r="E1359" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1360">
@@ -29038,7 +29038,7 @@
         </is>
       </c>
       <c r="E1362" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1363">
@@ -29059,7 +29059,7 @@
         </is>
       </c>
       <c r="E1363" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1364">
@@ -29269,7 +29269,7 @@
         </is>
       </c>
       <c r="E1373" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1374">
@@ -29374,7 +29374,7 @@
         </is>
       </c>
       <c r="E1378" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1379">
@@ -29458,7 +29458,7 @@
         </is>
       </c>
       <c r="E1382" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1383">
@@ -29626,7 +29626,7 @@
         </is>
       </c>
       <c r="E1390" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1391">
@@ -29836,7 +29836,7 @@
         </is>
       </c>
       <c r="E1400" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1401">
@@ -29983,7 +29983,7 @@
         </is>
       </c>
       <c r="E1407" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1408">
@@ -30151,7 +30151,7 @@
         </is>
       </c>
       <c r="E1415" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1416">
@@ -30403,7 +30403,7 @@
         </is>
       </c>
       <c r="E1427" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1428">
@@ -30571,7 +30571,7 @@
         </is>
       </c>
       <c r="E1435" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1436">
@@ -30865,7 +30865,7 @@
         </is>
       </c>
       <c r="E1449" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1450">
@@ -31033,7 +31033,7 @@
         </is>
       </c>
       <c r="E1457" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1458">
@@ -31138,7 +31138,7 @@
         </is>
       </c>
       <c r="E1462" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1463">
@@ -31222,7 +31222,7 @@
         </is>
       </c>
       <c r="E1466" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1467">
@@ -31264,7 +31264,7 @@
         </is>
       </c>
       <c r="E1468" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1469">
@@ -31390,7 +31390,7 @@
         </is>
       </c>
       <c r="E1474" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1475">
@@ -31474,7 +31474,7 @@
         </is>
       </c>
       <c r="E1478" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1479">
@@ -31495,7 +31495,7 @@
         </is>
       </c>
       <c r="E1479" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1480">
@@ -31747,7 +31747,7 @@
         </is>
       </c>
       <c r="E1491" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1492">
@@ -32041,7 +32041,7 @@
         </is>
       </c>
       <c r="E1505" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1506">
@@ -32083,7 +32083,7 @@
         </is>
       </c>
       <c r="E1507" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1508">
@@ -32209,7 +32209,7 @@
         </is>
       </c>
       <c r="E1513" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1514">
@@ -32503,7 +32503,7 @@
         </is>
       </c>
       <c r="E1527" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1528">
@@ -33028,7 +33028,7 @@
         </is>
       </c>
       <c r="E1552" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1553">
@@ -33091,7 +33091,7 @@
         </is>
       </c>
       <c r="E1555" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1556">
@@ -33112,7 +33112,7 @@
         </is>
       </c>
       <c r="E1556" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1557">
@@ -33259,7 +33259,7 @@
         </is>
       </c>
       <c r="E1563" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1564">
@@ -33532,7 +33532,7 @@
         </is>
       </c>
       <c r="E1576" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1577">
@@ -33616,7 +33616,7 @@
         </is>
       </c>
       <c r="E1580" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1581">
@@ -33637,7 +33637,7 @@
         </is>
       </c>
       <c r="E1581" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1582">
@@ -33952,7 +33952,7 @@
         </is>
       </c>
       <c r="E1596" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1597">
@@ -34204,7 +34204,7 @@
         </is>
       </c>
       <c r="E1608" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1609">
@@ -34225,7 +34225,7 @@
         </is>
       </c>
       <c r="E1609" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1610">
@@ -34372,7 +34372,7 @@
         </is>
       </c>
       <c r="E1616" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1617">
@@ -34519,7 +34519,7 @@
         </is>
       </c>
       <c r="E1623" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1624">
@@ -34645,7 +34645,7 @@
         </is>
       </c>
       <c r="E1629" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1630">
@@ -34813,7 +34813,7 @@
         </is>
       </c>
       <c r="E1637" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1638">
@@ -34834,7 +34834,7 @@
         </is>
       </c>
       <c r="E1638" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1639">
@@ -35170,7 +35170,7 @@
         </is>
       </c>
       <c r="E1654" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1655">
@@ -35380,7 +35380,7 @@
         </is>
       </c>
       <c r="E1664" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1665">
@@ -35401,7 +35401,7 @@
         </is>
       </c>
       <c r="E1665" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1666">
@@ -35926,7 +35926,7 @@
         </is>
       </c>
       <c r="E1690" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1691">
@@ -36136,7 +36136,7 @@
         </is>
       </c>
       <c r="E1700" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1701">
@@ -36367,7 +36367,7 @@
         </is>
       </c>
       <c r="E1711" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1712">
@@ -36934,7 +36934,7 @@
         </is>
       </c>
       <c r="E1738" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1739">
@@ -37081,7 +37081,7 @@
         </is>
       </c>
       <c r="E1745" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1746">
@@ -37144,7 +37144,7 @@
         </is>
       </c>
       <c r="E1748" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1749">
@@ -37186,7 +37186,7 @@
         </is>
       </c>
       <c r="E1750" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1751">
@@ -37228,7 +37228,7 @@
         </is>
       </c>
       <c r="E1752" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1753">
@@ -37270,7 +37270,7 @@
         </is>
       </c>
       <c r="E1754" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1755">
@@ -37312,7 +37312,7 @@
         </is>
       </c>
       <c r="E1756" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1757">
@@ -37354,7 +37354,7 @@
         </is>
       </c>
       <c r="E1758" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1759">
@@ -37564,7 +37564,7 @@
         </is>
       </c>
       <c r="E1768" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1769">
@@ -37774,7 +37774,7 @@
         </is>
       </c>
       <c r="E1778" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1779">
@@ -37837,7 +37837,7 @@
         </is>
       </c>
       <c r="E1781" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1782">
@@ -38362,7 +38362,7 @@
         </is>
       </c>
       <c r="E1806" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1807">
@@ -38719,7 +38719,7 @@
         </is>
       </c>
       <c r="E1823" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1824">
@@ -38803,7 +38803,7 @@
         </is>
       </c>
       <c r="E1827" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1828">
@@ -38845,7 +38845,7 @@
         </is>
       </c>
       <c r="E1829" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1830">
@@ -38929,7 +38929,7 @@
         </is>
       </c>
       <c r="E1833" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1834">
@@ -38992,7 +38992,7 @@
         </is>
       </c>
       <c r="E1836" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1837">
@@ -39076,7 +39076,7 @@
         </is>
       </c>
       <c r="E1840" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1841">
@@ -39097,7 +39097,7 @@
         </is>
       </c>
       <c r="E1841" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1842">
@@ -39118,7 +39118,7 @@
         </is>
       </c>
       <c r="E1842" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1843">
@@ -39307,7 +39307,7 @@
         </is>
       </c>
       <c r="E1851" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1852">
@@ -39433,7 +39433,7 @@
         </is>
       </c>
       <c r="E1857" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1858">
@@ -39748,7 +39748,7 @@
         </is>
       </c>
       <c r="E1872" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1873">
@@ -39853,7 +39853,7 @@
         </is>
       </c>
       <c r="E1877" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1878">
@@ -40126,7 +40126,7 @@
         </is>
       </c>
       <c r="E1890" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1891">
@@ -40231,7 +40231,7 @@
         </is>
       </c>
       <c r="E1895" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1896">
@@ -40273,7 +40273,7 @@
         </is>
       </c>
       <c r="E1897" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1898">
@@ -40378,7 +40378,7 @@
         </is>
       </c>
       <c r="E1902" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1903">
@@ -40525,7 +40525,7 @@
         </is>
       </c>
       <c r="E1909" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1910">
@@ -40567,7 +40567,7 @@
         </is>
       </c>
       <c r="E1911" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1912">
@@ -40588,7 +40588,7 @@
         </is>
       </c>
       <c r="E1912" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1913">
@@ -40672,7 +40672,7 @@
         </is>
       </c>
       <c r="E1916" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1917">
@@ -40840,7 +40840,7 @@
         </is>
       </c>
       <c r="E1924" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1925">
@@ -40903,7 +40903,7 @@
         </is>
       </c>
       <c r="E1927" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1928">
@@ -40987,7 +40987,7 @@
         </is>
       </c>
       <c r="E1931" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1932">
@@ -41050,7 +41050,7 @@
         </is>
       </c>
       <c r="E1934" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1935">
@@ -41092,7 +41092,7 @@
         </is>
       </c>
       <c r="E1936" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1937">
@@ -41197,7 +41197,7 @@
         </is>
       </c>
       <c r="E1941" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1942">
@@ -41302,7 +41302,7 @@
         </is>
       </c>
       <c r="E1946" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1947">
@@ -41659,7 +41659,7 @@
         </is>
       </c>
       <c r="E1963" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1964">
@@ -41701,7 +41701,7 @@
         </is>
       </c>
       <c r="E1965" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1966">
@@ -41890,7 +41890,7 @@
         </is>
       </c>
       <c r="E1974" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1975">
@@ -41974,7 +41974,7 @@
         </is>
       </c>
       <c r="E1978" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1979">
@@ -42289,7 +42289,7 @@
         </is>
       </c>
       <c r="E1993" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1994">
@@ -42331,7 +42331,7 @@
         </is>
       </c>
       <c r="E1995" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1996">
@@ -42478,7 +42478,7 @@
         </is>
       </c>
       <c r="E2002" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2003">
@@ -42541,7 +42541,7 @@
         </is>
       </c>
       <c r="E2005" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2006">
@@ -42583,7 +42583,7 @@
         </is>
       </c>
       <c r="E2007" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2008">
@@ -42898,7 +42898,7 @@
         </is>
       </c>
       <c r="E2022" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2023">
@@ -43066,7 +43066,7 @@
         </is>
       </c>
       <c r="E2030" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2031">
@@ -43444,7 +43444,7 @@
         </is>
       </c>
       <c r="E2048" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2049">
@@ -43465,7 +43465,7 @@
         </is>
       </c>
       <c r="E2049" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2050">
@@ -43570,7 +43570,7 @@
         </is>
       </c>
       <c r="E2054" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2055">
@@ -44242,7 +44242,7 @@
         </is>
       </c>
       <c r="E2086" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2087">
@@ -44284,7 +44284,7 @@
         </is>
       </c>
       <c r="E2088" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2089">
@@ -44389,7 +44389,7 @@
         </is>
       </c>
       <c r="E2093" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2094">
@@ -44578,7 +44578,7 @@
         </is>
       </c>
       <c r="E2102" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2103">
@@ -44788,7 +44788,7 @@
         </is>
       </c>
       <c r="E2112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2113">
@@ -44893,7 +44893,7 @@
         </is>
       </c>
       <c r="E2117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2118">
@@ -44914,7 +44914,7 @@
         </is>
       </c>
       <c r="E2118" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2119">
@@ -45334,7 +45334,7 @@
         </is>
       </c>
       <c r="E2138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2139">
@@ -45565,7 +45565,7 @@
         </is>
       </c>
       <c r="E2149" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2150">
@@ -45607,7 +45607,7 @@
         </is>
       </c>
       <c r="E2151" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2152">
@@ -45754,7 +45754,7 @@
         </is>
       </c>
       <c r="E2158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2159">
@@ -45775,7 +45775,7 @@
         </is>
       </c>
       <c r="E2159" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2160">
@@ -45817,7 +45817,7 @@
         </is>
       </c>
       <c r="E2161" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2162">
@@ -45901,7 +45901,7 @@
         </is>
       </c>
       <c r="E2165" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2166">
@@ -46552,7 +46552,7 @@
         </is>
       </c>
       <c r="E2196" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2197">
@@ -46615,7 +46615,7 @@
         </is>
       </c>
       <c r="E2199" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2200">
@@ -46741,7 +46741,7 @@
         </is>
       </c>
       <c r="E2205" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2206">
@@ -46909,7 +46909,7 @@
         </is>
       </c>
       <c r="E2213" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2214">
@@ -47035,7 +47035,7 @@
         </is>
       </c>
       <c r="E2219" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2220">
@@ -47098,7 +47098,7 @@
         </is>
       </c>
       <c r="E2222" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2223">
@@ -47119,7 +47119,7 @@
         </is>
       </c>
       <c r="E2223" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2224">
@@ -47329,7 +47329,7 @@
         </is>
       </c>
       <c r="E2233" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2234">
@@ -47371,7 +47371,7 @@
         </is>
       </c>
       <c r="E2235" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2236">
@@ -47455,7 +47455,7 @@
         </is>
       </c>
       <c r="E2239" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2240">
@@ -47707,7 +47707,7 @@
         </is>
       </c>
       <c r="E2251" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2252">
@@ -48211,7 +48211,7 @@
         </is>
       </c>
       <c r="E2275" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2276">
@@ -48253,7 +48253,7 @@
         </is>
       </c>
       <c r="E2277" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2278">
@@ -48400,7 +48400,7 @@
         </is>
       </c>
       <c r="E2284" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2285">
@@ -48568,7 +48568,7 @@
         </is>
       </c>
       <c r="E2292" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2293">
@@ -48652,7 +48652,7 @@
         </is>
       </c>
       <c r="E2296" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2297">
@@ -49030,7 +49030,7 @@
         </is>
       </c>
       <c r="E2314" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2315">
@@ -49072,7 +49072,7 @@
         </is>
       </c>
       <c r="E2316" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2317">
@@ -49093,7 +49093,7 @@
         </is>
       </c>
       <c r="E2317" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2318">
@@ -49156,7 +49156,7 @@
         </is>
       </c>
       <c r="E2320" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2321">
@@ -49177,7 +49177,7 @@
         </is>
       </c>
       <c r="E2321" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2322">
@@ -49450,7 +49450,7 @@
         </is>
       </c>
       <c r="E2334" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2335">
@@ -49492,7 +49492,7 @@
         </is>
       </c>
       <c r="E2336" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2337">
@@ -49513,7 +49513,7 @@
         </is>
       </c>
       <c r="E2337" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2338">
@@ -49597,7 +49597,7 @@
         </is>
       </c>
       <c r="E2341" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2342">
@@ -49639,7 +49639,7 @@
         </is>
       </c>
       <c r="E2343" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2344">
@@ -49828,7 +49828,7 @@
         </is>
       </c>
       <c r="E2352" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2353">
@@ -49891,7 +49891,7 @@
         </is>
       </c>
       <c r="E2355" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2356">
@@ -49912,7 +49912,7 @@
         </is>
       </c>
       <c r="E2356" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2357">
@@ -49933,7 +49933,7 @@
         </is>
       </c>
       <c r="E2357" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2358">
@@ -50206,7 +50206,7 @@
         </is>
       </c>
       <c r="E2370" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2371">
@@ -50416,7 +50416,7 @@
         </is>
       </c>
       <c r="E2380" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2381">
@@ -50500,7 +50500,7 @@
         </is>
       </c>
       <c r="E2384" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2385">
@@ -50521,7 +50521,7 @@
         </is>
       </c>
       <c r="E2385" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2386">
@@ -50689,7 +50689,7 @@
         </is>
       </c>
       <c r="E2393" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2394">
@@ -50773,7 +50773,7 @@
         </is>
       </c>
       <c r="E2397" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2398">
@@ -50836,7 +50836,7 @@
         </is>
       </c>
       <c r="E2400" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2401">
@@ -50962,7 +50962,7 @@
         </is>
       </c>
       <c r="E2406" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2407">
@@ -51046,7 +51046,7 @@
         </is>
       </c>
       <c r="E2410" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2411">
@@ -51256,7 +51256,7 @@
         </is>
       </c>
       <c r="E2420" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2421">
@@ -51340,7 +51340,7 @@
         </is>
       </c>
       <c r="E2424" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2425">
@@ -51571,7 +51571,7 @@
         </is>
       </c>
       <c r="E2435" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2436">
@@ -51655,7 +51655,7 @@
         </is>
       </c>
       <c r="E2439" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2440">
@@ -51676,7 +51676,7 @@
         </is>
       </c>
       <c r="E2440" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2441">
@@ -51781,7 +51781,7 @@
         </is>
       </c>
       <c r="E2445" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2446">
@@ -51865,7 +51865,7 @@
         </is>
       </c>
       <c r="E2449" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2450">
@@ -51949,7 +51949,7 @@
         </is>
       </c>
       <c r="E2453" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2454">
@@ -52348,7 +52348,7 @@
         </is>
       </c>
       <c r="E2472" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2473">
@@ -52537,7 +52537,7 @@
         </is>
       </c>
       <c r="E2481" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2482">
@@ -52663,7 +52663,7 @@
         </is>
       </c>
       <c r="E2487" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2488">
@@ -52768,7 +52768,7 @@
         </is>
       </c>
       <c r="E2492" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2493">
@@ -52852,7 +52852,7 @@
         </is>
       </c>
       <c r="E2496" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2497">
@@ -52894,7 +52894,7 @@
         </is>
       </c>
       <c r="E2498" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2499">
@@ -52915,7 +52915,7 @@
         </is>
       </c>
       <c r="E2499" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2500">
@@ -52936,7 +52936,7 @@
         </is>
       </c>
       <c r="E2500" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2501">
@@ -53062,7 +53062,7 @@
         </is>
       </c>
       <c r="E2506" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2507">
@@ -53209,7 +53209,7 @@
         </is>
       </c>
       <c r="E2513" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2514">
@@ -53251,7 +53251,7 @@
         </is>
       </c>
       <c r="E2515" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2516">
@@ -53461,7 +53461,7 @@
         </is>
       </c>
       <c r="E2525" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2526">
@@ -53692,7 +53692,7 @@
         </is>
       </c>
       <c r="E2536" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2537">
@@ -53713,7 +53713,7 @@
         </is>
       </c>
       <c r="E2537" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2538">
@@ -53923,7 +53923,7 @@
         </is>
       </c>
       <c r="E2547" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2548">
@@ -54322,7 +54322,7 @@
         </is>
       </c>
       <c r="E2566" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2567">
@@ -54574,7 +54574,7 @@
         </is>
       </c>
       <c r="E2578" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2579">
@@ -54868,7 +54868,7 @@
         </is>
       </c>
       <c r="E2592" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2593">
@@ -54889,7 +54889,7 @@
         </is>
       </c>
       <c r="E2593" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2594">
@@ -55435,7 +55435,7 @@
         </is>
       </c>
       <c r="E2619" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2620">
@@ -55519,7 +55519,7 @@
         </is>
       </c>
       <c r="E2623" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2624">
@@ -55708,7 +55708,7 @@
         </is>
       </c>
       <c r="E2632" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2633">
@@ -55771,7 +55771,7 @@
         </is>
       </c>
       <c r="E2635" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2636">
@@ -55813,7 +55813,7 @@
         </is>
       </c>
       <c r="E2637" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2638">
@@ -56002,7 +56002,7 @@
         </is>
       </c>
       <c r="E2646" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2647">
@@ -56086,7 +56086,7 @@
         </is>
       </c>
       <c r="E2650" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2651">
@@ -56107,7 +56107,7 @@
         </is>
       </c>
       <c r="E2651" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2652">
@@ -56170,7 +56170,7 @@
         </is>
       </c>
       <c r="E2654" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2655">
@@ -56233,7 +56233,7 @@
         </is>
       </c>
       <c r="E2657" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2658">
@@ -56359,7 +56359,7 @@
         </is>
       </c>
       <c r="E2663" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>